<commit_message>
Update DD & Code API
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
+++ b/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng quan" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="139">
   <si>
     <t>Tác giả:</t>
   </si>
@@ -127,9 +127,6 @@
     <t>?diachi="abc"</t>
   </si>
   <si>
-    <t>Tìm kiếm cư trú theo đỉa chỉ cư trú</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -437,6 +434,15 @@
   </si>
   <si>
     <t>/{id}</t>
+  </si>
+  <si>
+    <t>Tìm kiếm cư trú theo địa chỉ cư trú</t>
+  </si>
+  <si>
+    <t>updateNguoiDung(id, nguoiDung)</t>
+  </si>
+  <si>
+    <t>Cập nhật người dùng theo id</t>
   </si>
 </sst>
 </file>
@@ -919,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,7 +979,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="5">
-        <v>43365</v>
+        <v>43366</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -987,13 +993,13 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="45" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.88671875" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.77734375" style="3" bestFit="1" customWidth="1"/>
@@ -1018,7 +1024,7 @@
         <v>14</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1038,7 +1044,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1046,7 +1052,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -1055,10 +1061,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1066,7 +1072,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
@@ -1078,7 +1084,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1086,7 +1092,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
@@ -1098,7 +1104,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1106,7 +1112,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
@@ -1118,7 +1124,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1126,7 +1132,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
@@ -1138,7 +1144,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1146,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -1158,7 +1164,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1166,7 +1172,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
@@ -1178,7 +1184,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1186,7 +1192,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -1198,7 +1204,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1206,19 +1212,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1226,19 +1232,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1246,19 +1252,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1266,19 +1272,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F14" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1286,19 +1292,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="F15" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1310,10 +1316,8 @@
     <hyperlink ref="F6" location="CuTruDO" display="[CuTru]"/>
     <hyperlink ref="F8" location="CuTruDO" display="[CuTru]"/>
     <hyperlink ref="F10" location="CuTruDO" display="[CuTru]"/>
-    <hyperlink ref="F12" location="CuTruDO" display="[CuTru]"/>
     <hyperlink ref="F7" location="CuTruDO" display="[CuTru]"/>
     <hyperlink ref="F9" location="CuTruDO" display="[CuTru]"/>
-    <hyperlink ref="F11" location="CuTruDO" display="[CuTru]"/>
     <hyperlink ref="F13" location="CuTruDO" display="CuTru"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1323,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1361,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -1370,7 +1374,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1378,16 +1382,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1395,16 +1399,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1412,16 +1416,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1429,16 +1433,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1446,16 +1450,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1463,16 +1467,33 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>70</v>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1484,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1502,19 +1523,19 @@
   <sheetData>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" s="22"/>
     </row>
@@ -1525,184 +1546,184 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C26" s="22"/>
     </row>
@@ -1713,178 +1734,178 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new API, Added home view, Update DD
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
+++ b/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng quan" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
   <definedNames>
     <definedName name="CuTruDO">'Data Object'!$B$5</definedName>
     <definedName name="NguoiDungDO">'Data Object'!$B$25</definedName>
+    <definedName name="TrangChuDO">'Data Object'!$B$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="153">
   <si>
     <t>Tác giả:</t>
   </si>
@@ -241,9 +242,6 @@
     <t>getCuTrusByPersonalAddress(diaChiDan)</t>
   </si>
   <si>
-    <t>カラム名</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -283,12 +281,6 @@
     <t>canBoId</t>
   </si>
   <si>
-    <t>説明</t>
-  </si>
-  <si>
-    <t>データ種別</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -358,9 +350,6 @@
     <t>Danh sách công dân</t>
   </si>
   <si>
-    <t>対象名</t>
-  </si>
-  <si>
     <t>Lưu thông tin cư trú</t>
   </si>
   <si>
@@ -373,9 +362,6 @@
     <t>NguoiDung</t>
   </si>
   <si>
-    <t>Lưu thông tin người dùng</t>
-  </si>
-  <si>
     <t>hoTen</t>
   </si>
   <si>
@@ -443,6 +429,63 @@
   </si>
   <si>
     <t>Cập nhật người dùng theo id</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Tên object</t>
+  </si>
+  <si>
+    <t>Tên param</t>
+  </si>
+  <si>
+    <t>Kiểu dữ liệu</t>
+  </si>
+  <si>
+    <t>Danh sách object và diễn giải</t>
+  </si>
+  <si>
+    <t>TrangChu</t>
+  </si>
+  <si>
+    <t>tongSo</t>
+  </si>
+  <si>
+    <t>dangKyHomNay</t>
+  </si>
+  <si>
+    <t>choDuyet</t>
+  </si>
+  <si>
+    <t>hetHan</t>
+  </si>
+  <si>
+    <t>cuTrus</t>
+  </si>
+  <si>
+    <t>Tổng số cư trú</t>
+  </si>
+  <si>
+    <t>Số lượt đăng ký hôm nay</t>
+  </si>
+  <si>
+    <t>Số cư trú chờ duyệt (chưa duyệt)</t>
+  </si>
+  <si>
+    <t>Lấy thông tin tóm tắt cho trang chủ</t>
+  </si>
+  <si>
+    <t>getTrangChuInfo()</t>
+  </si>
+  <si>
+    <t>Danh sách cư trú chưa duyệt</t>
+  </si>
+  <si>
+    <t>Số cư trú đã hết hạn</t>
+  </si>
+  <si>
+    <t>/trangchu</t>
   </si>
 </sst>
 </file>
@@ -925,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -979,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="5">
-        <v>43366</v>
+        <v>43373</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -990,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1015,7 +1058,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>10</v>
@@ -1024,7 +1067,7 @@
         <v>14</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1044,7 +1087,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1061,10 +1104,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1084,7 +1127,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1104,7 +1147,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1124,7 +1167,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1144,7 +1187,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1164,7 +1207,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1184,7 +1227,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1204,7 +1247,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1221,10 +1264,10 @@
         <v>32</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1244,7 +1287,7 @@
         <v>31</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1264,7 +1307,7 @@
         <v>34</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1278,13 +1321,13 @@
         <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1298,13 +1341,33 @@
         <v>36</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1319,6 +1382,7 @@
     <hyperlink ref="F7" location="CuTruDO" display="[CuTru]"/>
     <hyperlink ref="F9" location="CuTruDO" display="[CuTru]"/>
     <hyperlink ref="F13" location="CuTruDO" display="CuTru"/>
+    <hyperlink ref="F16" location="TrangChuDO" display="TrangChu"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1388,7 +1452,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>55</v>
@@ -1484,16 +1548,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1503,17 +1567,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:C43"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24" style="3" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.21875" style="3" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="3"/>
     <col min="5" max="5" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="3" bestFit="1" customWidth="1"/>
@@ -1521,21 +1585,26 @@
     <col min="8" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C6" s="22"/>
     </row>
@@ -1546,184 +1615,184 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>114</v>
       </c>
       <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C26" s="22"/>
     </row>
@@ -1734,181 +1803,271 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="19"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="22"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="9"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new API Interface
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
+++ b/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="155">
   <si>
     <t>Tác giả:</t>
   </si>
@@ -486,6 +486,12 @@
   </si>
   <si>
     <t>/trangchu</t>
+  </si>
+  <si>
+    <t>searchCuTrus(loaiTimKiem, loaiCuTru, loaiTrangThai, loaiHan, timKiem)</t>
+  </si>
+  <si>
+    <t>Tìm kiếm cư trú theo bộ lọc (filter)</t>
   </si>
 </sst>
 </file>
@@ -655,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -684,6 +690,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1022,7 +1031,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="5">
-        <v>43373</v>
+        <v>43377</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -1033,16 +1042,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="45.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.88671875" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.77734375" style="3" bestFit="1" customWidth="1"/>
@@ -1368,6 +1377,26 @@
       </c>
       <c r="F16" s="24" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update DD & Backend logics
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
+++ b/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng quan" sheetId="1" r:id="rId1"/>
@@ -14,8 +14,8 @@
   </sheets>
   <definedNames>
     <definedName name="CuTruDO">'Data Object'!$B$5</definedName>
-    <definedName name="NguoiDungDO">'Data Object'!$B$25</definedName>
-    <definedName name="TrangChuDO">'Data Object'!$B$46</definedName>
+    <definedName name="NguoiDungDO">'Data Object'!$B$28</definedName>
+    <definedName name="TrangChuDO">'Data Object'!$B$49</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="160">
   <si>
     <t>Tác giả:</t>
   </si>
@@ -492,6 +492,21 @@
   </si>
   <si>
     <t>Tìm kiếm cư trú theo bộ lọc (filter)</t>
+  </si>
+  <si>
+    <t>Họ tên công dân của Cư Trú</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Email người đăng ký</t>
+  </si>
+  <si>
+    <t>diaChi</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1596,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1699,399 +1714,432 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>75</v>
+        <v>156</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>97</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>98</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B25" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B28" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="19"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
+      <c r="C28" s="19"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B29" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="22"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+      <c r="C29" s="22"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B31" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C31" s="17" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C42" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B46" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C46" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="18" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="23" t="s">
+      <c r="B49" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="19"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="20" t="s">
+      <c r="C49" s="19"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B50" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C47" s="22"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="9"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="11"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="15" t="s">
+      <c r="C50" s="22"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="9"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B52" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C52" s="17" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>109</v>
       </c>
       <c r="C53" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="12" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B57" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C57" s="14" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added "DangKyCuTru" page, Added "body-content" to global styles
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
+++ b/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1613,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update DD, implemented ChiTietCuTru, Duyet function
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
+++ b/Specifications (仕様書)/DD (詳細設計)/API Interface.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng quan" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="NguoiDungDO">'Data Object'!$B$28</definedName>
     <definedName name="TrangChuDO">'Data Object'!$B$50</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="160">
   <si>
     <t>Tác giả:</t>
   </si>
@@ -303,9 +303,6 @@
   </si>
   <si>
     <t>Lấy cư trú theo id</t>
-  </si>
-  <si>
-    <t>void</t>
   </si>
   <si>
     <t>Mã số cư trú</t>
@@ -679,7 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -688,9 +685,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -985,7 +979,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1062,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1085,7 +1079,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>10</v>
@@ -1113,7 +1107,7 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1133,7 +1127,7 @@
       <c r="E3" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1153,7 +1147,7 @@
       <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1173,7 +1167,7 @@
       <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1193,7 +1187,7 @@
       <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1213,7 +1207,7 @@
       <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1233,7 +1227,7 @@
       <c r="E8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1253,7 +1247,7 @@
       <c r="E9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1273,7 +1267,7 @@
       <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1291,9 +1285,9 @@
         <v>32</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1313,7 +1307,7 @@
       <c r="E12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1333,7 +1327,7 @@
       <c r="E13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="23" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1348,12 +1342,12 @@
         <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="23" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1368,13 +1362,13 @@
         <v>36</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>92</v>
+      <c r="F15" s="23" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1382,27 +1376,27 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>139</v>
+        <v>147</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>153</v>
+      <c r="B17" s="24" t="s">
+        <v>152</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>9</v>
@@ -1411,9 +1405,9 @@
         <v>11</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F17" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1431,6 +1425,7 @@
     <hyperlink ref="F13" location="CuTruDO" display="CuTru"/>
     <hyperlink ref="F16" location="TrangChuDO" display="TrangChu"/>
     <hyperlink ref="F14" location="CuTruDO" display="CuTru"/>
+    <hyperlink ref="F15" location="CuTruDO" display="CuTru"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1500,7 +1495,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>55</v>
@@ -1596,16 +1591,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1617,7 +1612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -1635,527 +1630,527 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="18"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="21"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="22" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="C50" s="18"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="21"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="10"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="19"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="B53" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="22"/>
-    </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="13" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="19"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C29" s="22"/>
-    </row>
-    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="C50" s="19"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C51" s="22"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="11"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
+      <c r="C54" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B54" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="11" t="s">
+      <c r="B55" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C55" s="11" t="s">
+      <c r="B56" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="9" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B56" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="9" t="s">
+      <c r="B57" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="14" t="s">
-        <v>150</v>
+      <c r="C58" s="13" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>